<commit_message>
Not Completed Bugfixing for Bug with ID 1
</commit_message>
<xml_diff>
--- a/Planing/Bugs.xlsx
+++ b/Planing/Bugs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Bug</t>
   </si>
@@ -80,6 +80,33 @@
   </si>
   <si>
     <t>Moonjump-Bug</t>
+  </si>
+  <si>
+    <t>Infinity-Jump-Bug</t>
+  </si>
+  <si>
+    <t>Mögliche Lösung</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>das GameObject Inventory_UI und Inventory_Main_Driver werden 2x geladen checken ob es schon geladen ist</t>
+  </si>
+  <si>
+    <t>Checken ob GameObject schon erstellt wurde</t>
+  </si>
+  <si>
+    <t>Entsteht wenn man bei einem Hinweis</t>
+  </si>
+  <si>
+    <t>Bugged-Knockback</t>
+  </si>
+  <si>
+    <t>Entsteht wenn Player schaden nimmt</t>
+  </si>
+  <si>
+    <t>Wenn der Player schaden erleidet</t>
   </si>
 </sst>
 </file>
@@ -465,11 +492,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A2:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -478,365 +503,421 @@
     <col min="4" max="4" width="49.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="100.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="2" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="G2" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E4" s="1">
         <v>0</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="G5" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1" t="s">
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="B8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>7</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>8</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Started Stoney Mini-Boss in Cave
</commit_message>
<xml_diff>
--- a/Planing/Bugs.xlsx
+++ b/Planing/Bugs.xlsx
@@ -506,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>